<commit_message>
feat: lógica para cargue despachos y remisiones
</commit_message>
<xml_diff>
--- a/apps/static/cargues_masivos/ejemplo_despachos.xlsx
+++ b/apps/static/cargues_masivos/ejemplo_despachos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SINTRA\apps\templates\cargues_masivos\ejemplos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SINTRA\apps\static\cargues_masivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20973C2-FEEB-4EF1-B2F4-5A88CE62903E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A323C5E5-27C5-488F-8933-19A969B24E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,16 +25,52 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>DESPACHOS</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+  <si>
+    <t>CÓDIGO OC</t>
+  </si>
+  <si>
+    <t>REFERENCIA</t>
+  </si>
+  <si>
+    <t>CANTIDAD DESPACHADA</t>
+  </si>
+  <si>
+    <t>FECHA DESPACHO</t>
+  </si>
+  <si>
+    <t>OCAM-63-2021-115</t>
+  </si>
+  <si>
+    <t>CI1-U</t>
+  </si>
+  <si>
+    <t>07/ene/2022</t>
+  </si>
+  <si>
+    <t>OCAM-57-2021-115</t>
+  </si>
+  <si>
+    <t>CIH1-L</t>
+  </si>
+  <si>
+    <t>06/ene/2021</t>
+  </si>
+  <si>
+    <t>CIH1-XXL</t>
+  </si>
+  <si>
+    <t>11/ene/2022</t>
+  </si>
+  <si>
+    <t># REMISIÓN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -42,13 +78,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -63,8 +113,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -345,17 +401,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2">
+        <v>139</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2">
+        <v>32</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2">
+        <v>51</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>